<commit_message>
CAMBIOS EN LA DOCUMENTACIÓN
</commit_message>
<xml_diff>
--- a/documentacion/Product Backlog detallado.xlsx
+++ b/documentacion/Product Backlog detallado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aplicaciones Informática II\proyecto_6827\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\CartaDigital\icard_server\icard\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFFD0F1-5424-4B9B-A6E4-CE0CB6E84FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E46FE7-4651-4D9A-A648-6B299EFBEB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD518A79-2D44-421E-8D6F-D6CB2008D04E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -75,9 +75,6 @@
     <t>SPRINT 1</t>
   </si>
   <si>
-    <t>Planificado</t>
-  </si>
-  <si>
     <t>2 horas</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>14 horas</t>
-  </si>
-  <si>
     <t>Se va a utilizar la plataforma GitHub para de esta manera permitir al docente visualizar todos los cambios que se realizan a lo largo del proyecto.</t>
   </si>
   <si>
@@ -106,22 +100,155 @@
   </si>
   <si>
     <t>4 horas</t>
+  </si>
+  <si>
+    <t>HI-TE-04</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>Se implementará un sistema de rutas la cual necesitará de varias librerías como React Router Dom v6, y también se implementará la ruta de Error404 la cuál mostrará un comentario de error al intentar entrar en una ruta no válida</t>
+  </si>
+  <si>
+    <t>Implementación del sistema de rutas del proyecto</t>
+  </si>
+  <si>
+    <t>HI-TE-05</t>
+  </si>
+  <si>
+    <t>Se implementará un sistema de usuarios con su respectiva autenticación en la cuál se implementarán los CRUDS de usuarios y un log in para los mismos</t>
+  </si>
+  <si>
+    <t>Implementación del modelado de usuarios con el log-in</t>
+  </si>
+  <si>
+    <t>6 horas</t>
+  </si>
+  <si>
+    <t>HI-TE-06</t>
+  </si>
+  <si>
+    <t>Se implementará el Panel de Administrador el cual contendrá reestricción de usuarios sin rol de staff al momento de ingresar al panel de los usuarios del sistema</t>
+  </si>
+  <si>
+    <t>Implementación de la interfaz del panel de administrador</t>
+  </si>
+  <si>
+    <t>HI-TE-07</t>
+  </si>
+  <si>
+    <t>HI-TE-08</t>
+  </si>
+  <si>
+    <t>HI-TE-09</t>
+  </si>
+  <si>
+    <t>HI-TE-10</t>
+  </si>
+  <si>
+    <t>HI-TE-11</t>
+  </si>
+  <si>
+    <t>HI-TE-12</t>
+  </si>
+  <si>
+    <t>HI-TE-13</t>
+  </si>
+  <si>
+    <t>HI-TE-14</t>
+  </si>
+  <si>
+    <t>HI-TE-15</t>
+  </si>
+  <si>
+    <t>Implementación del modelo de categorías</t>
+  </si>
+  <si>
+    <t>8 horas</t>
+  </si>
+  <si>
+    <t>Se implementará el módulo de categorías de los productos del restaurante, en el cuál se implementarán los CRUDS del modelo</t>
+  </si>
+  <si>
+    <t>Se implementará el módulo de productos existentes en el restaurante, y sus respectivos CRUDS.</t>
+  </si>
+  <si>
+    <t>Implementación del modelado de los productos</t>
+  </si>
+  <si>
+    <t>5 horas</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>3 horas</t>
+  </si>
+  <si>
+    <t>9 horas</t>
+  </si>
+  <si>
+    <t>7 horas</t>
+  </si>
+  <si>
+    <t>Se implementará el módulo de las mesas del restaurant el cuál tendrá su respectivo CRUD y además un QR mediante el cuál se podrá acceder a una mesa en específico</t>
+  </si>
+  <si>
+    <t>Implementación del modelado de las mesas</t>
+  </si>
+  <si>
+    <t>Se implementará un sistema de pagos el cuál tendrá el tipo de pago que el cliente va a realizar sea efectivo o por tarjeta</t>
+  </si>
+  <si>
+    <t>Implementación del sistema de pedidos</t>
+  </si>
+  <si>
+    <t>Se implementará un sistema el cual contendrá los detalles de las mesas existentes en restaurante y se identificará fácilmente cual mesa está disponible, o cual está ocupada, etc</t>
+  </si>
+  <si>
+    <t>Implementación de un sistema del detalle de las mesas</t>
+  </si>
+  <si>
+    <t>Implementación del sistema de pagos</t>
+  </si>
+  <si>
+    <t>Se implementará un sistema de pedidos el cuál se encargará de gestionar eficientemente las solicitudes de los clientes del restaurant</t>
+  </si>
+  <si>
+    <t>Se implementará una pestaña de historial de pedidos el cual mostrará el historial de pedidos realizados en el restaurant</t>
+  </si>
+  <si>
+    <t>Implementación de la pestaña de historial de pedidos</t>
+  </si>
+  <si>
+    <t>Se implementará una interfaz para el cliente el cual contendrán las mismas funcionalidades que la parte administrativa del restaurante</t>
+  </si>
+  <si>
+    <t>Implementación de interfaz del cliente</t>
+  </si>
+  <si>
+    <t>12 horas</t>
+  </si>
+  <si>
+    <t>Implementación del QR en la parte administrativa del sistema</t>
+  </si>
+  <si>
+    <t>Implementación del QR</t>
+  </si>
+  <si>
+    <t>1 hora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,6 +268,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -221,32 +362,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,7 +712,7 @@
   <dimension ref="F1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,409 +727,577 @@
   </cols>
   <sheetData>
     <row r="1" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F6" s="5" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="6:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="6:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="K8" s="7"/>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="6:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="6:12" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="J9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="6" t="s">
+    </row>
+    <row r="10" spans="6:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="6:12" ht="51" x14ac:dyDescent="0.25">
-      <c r="F9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="L10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="K12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="6:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="F21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
     </row>
     <row r="23" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
     </row>
     <row r="25" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
     </row>
     <row r="27" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
     </row>
     <row r="28" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
     </row>
     <row r="29" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
     </row>
     <row r="31" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
     </row>
     <row r="32" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
     </row>
     <row r="35" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
     </row>
     <row r="38" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
     </row>
     <row r="40" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
@@ -1058,37 +1372,38 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
     </row>
     <row r="49" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:L4"/>
     <mergeCell ref="K7:K9"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>